<commit_message>
Agrega tabla alturas libres piso
</commit_message>
<xml_diff>
--- a/Tarea 03/Cubicaciones.xlsx
+++ b/Tarea 03/Cubicaciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5ADB6D16-1CD5-42DE-8A70-0FA7F4B5E17C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,15 +19,93 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{BD13D700-ADAE-46F7-8CAB-9A25E47FDE3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Investigar</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>$\gamma_{Hormigon}$</t>
+  </si>
+  <si>
+    <t>Densidad [$T/m^3$]</t>
+  </si>
+  <si>
+    <t>$\gamma_{Sobrelosa}$</t>
+  </si>
+  <si>
+    <t>$\gamma_{Estuco}$</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>Densidades de cada elemento</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +124,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +433,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Termina cálculo cubicación losas
</commit_message>
<xml_diff>
--- a/Tarea 03/Cubicaciones.xlsx
+++ b/Tarea 03/Cubicaciones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C7A70FD-FA58-4F66-816C-457593C4070D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F56E787A-D088-43BE-9D78-923704147FA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cubicaciones" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,103 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{BD13D700-ADAE-46F7-8CAB-9A25E47FDE3D}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{24553EEE-1DF4-469B-8DCD-AEC795EA3A2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Área de losa que tiene sobrelosa+eslucido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{4821EEAA-CF5D-4F0C-8992-F14CAE725CA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Corrección muro+viga</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{EAB6CE26-8075-4BD5-90F8-3A2648A64422}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Descuento áreas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{48E05DE0-C362-4F50-9D77-F1CA451ECCA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Área total estacionamiento</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{BD13D700-ADAE-46F7-8CAB-9A25E47FDE3D}">
       <text>
         <r>
           <rPr>
@@ -89,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Estuco</t>
   </si>
@@ -184,6 +280,9 @@
     <t>[T/cm^2]</t>
   </si>
   <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
     <t>Alosa</t>
   </si>
   <si>
@@ -203,6 +302,54 @@
   </si>
   <si>
     <t>Alturas libres de pisos (entre losas)</t>
+  </si>
+  <si>
+    <t>Descuento muro/viga</t>
+  </si>
+  <si>
+    <t>Área losa interior</t>
+  </si>
+  <si>
+    <t>Área estacionamientos</t>
+  </si>
+  <si>
+    <t>Losas</t>
+  </si>
+  <si>
+    <t>Espesor (m)</t>
+  </si>
+  <si>
+    <t>Área losa interior final (m2)</t>
+  </si>
+  <si>
+    <t>Área losa estacionamiento final (m2)</t>
+  </si>
+  <si>
+    <t>Peso total (T)</t>
+  </si>
+  <si>
+    <t>Espesor (cm)</t>
+  </si>
+  <si>
+    <t>Piso 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piso 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piso 3 </t>
+  </si>
+  <si>
+    <t>Piso Tipo</t>
+  </si>
+  <si>
+    <t>Cubierta</t>
+  </si>
+  <si>
+    <t>Espesor losas</t>
+  </si>
+  <si>
+    <t>$\gamma_{Eslucido}$</t>
   </si>
 </sst>
 </file>
@@ -212,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +395,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +441,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -446,6 +631,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -506,17 +702,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -616,65 +861,176 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -968,299 +1324,1178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="52"/>
+    <col min="6" max="6" width="13.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="52"/>
+    <col min="9" max="9" width="7.6640625" style="52" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="52" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="52" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="52" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" style="52" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="52" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="52" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="52" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="52"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="51"/>
+    </row>
+    <row r="3" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="H3" s="87" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="89" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="55">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="56">
+        <v>24</v>
+      </c>
+      <c r="F4" s="57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H4" s="58">
+        <f>E4</f>
+        <v>24</v>
+      </c>
+      <c r="I4" s="58">
+        <f>C21</f>
+        <v>0.16</v>
+      </c>
+      <c r="J4" s="70">
+        <v>68.697999999999993</v>
+      </c>
+      <c r="K4" s="70">
+        <v>0</v>
+      </c>
+      <c r="L4" s="71">
+        <f>J4-K4</f>
+        <v>68.697999999999993</v>
+      </c>
+      <c r="M4" s="70">
+        <v>0</v>
+      </c>
+      <c r="N4" s="70">
+        <v>0</v>
+      </c>
+      <c r="O4" s="72">
+        <f>M4-N4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="73">
+        <f>L4*($C$4*I4+$C$6*$C$12+$C$7*$C$13)+I4*O4*$C$4</f>
+        <v>33.455925999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="59">
+        <v>2</v>
+      </c>
+      <c r="E5" s="60">
+        <v>23</v>
+      </c>
+      <c r="F5" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H5" s="81">
+        <f t="shared" ref="H5:H28" si="0">E5</f>
+        <v>23</v>
+      </c>
+      <c r="I5" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J5" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K5" s="82">
+        <v>0</v>
+      </c>
+      <c r="L5" s="83">
+        <f>J5-K5</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M5" s="82">
+        <v>0</v>
+      </c>
+      <c r="N5" s="82">
+        <v>0</v>
+      </c>
+      <c r="O5" s="84">
+        <f t="shared" ref="O5:O27" si="1">M5-N5</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="73">
+        <f t="shared" ref="P5:P27" si="2">L5*($C$4*I5+$C$6*$C$12+$C$7*$C$13)+I5*O5*$C$4</f>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="60">
+        <v>22</v>
+      </c>
+      <c r="F6" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H6" s="81">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I6" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J6" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K6" s="82">
+        <v>0</v>
+      </c>
+      <c r="L6" s="83">
+        <f>J6-K6</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M6" s="82">
+        <v>0</v>
+      </c>
+      <c r="N6" s="82">
+        <v>0</v>
+      </c>
+      <c r="O6" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="62">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="60">
+        <v>21</v>
+      </c>
+      <c r="F7" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H7" s="81">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I7" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J7" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K7" s="82">
+        <v>0</v>
+      </c>
+      <c r="L7" s="83">
+        <f>J7-K7</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M7" s="82">
+        <v>0</v>
+      </c>
+      <c r="N7" s="82">
+        <v>0</v>
+      </c>
+      <c r="O7" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E8" s="60">
+        <v>20</v>
+      </c>
+      <c r="F8" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H8" s="81">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I8" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J8" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K8" s="82">
+        <v>0</v>
+      </c>
+      <c r="L8" s="83">
+        <f>J8-K8</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M8" s="82">
+        <v>0</v>
+      </c>
+      <c r="N8" s="82">
+        <v>0</v>
+      </c>
+      <c r="O8" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="60">
+        <v>19</v>
+      </c>
+      <c r="F9" s="61">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H9" s="81">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="I9" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J9" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K9" s="82">
+        <v>0</v>
+      </c>
+      <c r="L9" s="83">
+        <f>J9-K9</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M9" s="82">
+        <v>0</v>
+      </c>
+      <c r="N9" s="82">
+        <v>0</v>
+      </c>
+      <c r="O9" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C10" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>24</v>
-      </c>
-      <c r="F4" s="55">
+      <c r="E10" s="60">
+        <v>18</v>
+      </c>
+      <c r="F10" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>23</v>
-      </c>
-      <c r="F5" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>22</v>
-      </c>
-      <c r="F6" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E7" s="3">
-        <v>21</v>
-      </c>
-      <c r="F7" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="3">
-        <v>20</v>
-      </c>
-      <c r="F8" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3">
-        <v>19</v>
-      </c>
-      <c r="F9" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="H10" s="81">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I10" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J10" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K10" s="82">
+        <v>0</v>
+      </c>
+      <c r="L10" s="83">
+        <f>J10-K10</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M10" s="82">
+        <v>0</v>
+      </c>
+      <c r="N10" s="82">
+        <v>0</v>
+      </c>
+      <c r="O10" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="55">
         <f>2.5/100</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E10" s="3">
-        <v>18</v>
-      </c>
-      <c r="F10" s="55">
+      <c r="E11" s="60">
+        <v>17</v>
+      </c>
+      <c r="F11" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
+      <c r="H11" s="81">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="I11" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J11" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K11" s="82">
+        <v>0</v>
+      </c>
+      <c r="L11" s="83">
+        <f>J11-K11</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M11" s="82">
+        <v>0</v>
+      </c>
+      <c r="N11" s="82">
+        <v>0</v>
+      </c>
+      <c r="O11" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="59">
         <f>5/100</f>
         <v>0.05</v>
       </c>
-      <c r="E11" s="3">
-        <v>17</v>
-      </c>
-      <c r="F11" s="55">
+      <c r="E12" s="60">
+        <v>16</v>
+      </c>
+      <c r="F12" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3">
-        <f>2/100</f>
-        <v>0.02</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="H12" s="81">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F12" s="55">
+      <c r="I12" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J12" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K12" s="82">
+        <v>0</v>
+      </c>
+      <c r="L12" s="83">
+        <f>J12-K12</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M12" s="82">
+        <v>0</v>
+      </c>
+      <c r="N12" s="82">
+        <v>0</v>
+      </c>
+      <c r="O12" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="62">
+        <v>0.03</v>
+      </c>
+      <c r="E13" s="60">
+        <v>15</v>
+      </c>
+      <c r="F13" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E13" s="3">
+      <c r="H13" s="81">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F13" s="55">
+      <c r="I13" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J13" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K13" s="82">
+        <v>0</v>
+      </c>
+      <c r="L13" s="83">
+        <f>J13-K13</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M13" s="82">
+        <v>0</v>
+      </c>
+      <c r="N13" s="82">
+        <v>0</v>
+      </c>
+      <c r="O13" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="60">
+        <v>14</v>
+      </c>
+      <c r="F14" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E14" s="3">
+      <c r="H14" s="81">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F14" s="55">
+      <c r="I14" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J14" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K14" s="82">
+        <v>0</v>
+      </c>
+      <c r="L14" s="83">
+        <f>J14-K14</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M14" s="82">
+        <v>0</v>
+      </c>
+      <c r="N14" s="82">
+        <v>0</v>
+      </c>
+      <c r="O14" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="60">
+        <v>13</v>
+      </c>
+      <c r="F15" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="3">
+      <c r="H15" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F15" s="55">
+      <c r="I15" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J15" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K15" s="82">
+        <v>0</v>
+      </c>
+      <c r="L15" s="83">
+        <f>J15-K15</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M15" s="82">
+        <v>0</v>
+      </c>
+      <c r="N15" s="82">
+        <v>0</v>
+      </c>
+      <c r="O15" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="60">
+        <v>12</v>
+      </c>
+      <c r="F16" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="3">
+      <c r="H16" s="81">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F16" s="55">
+      <c r="I16" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J16" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K16" s="82">
+        <v>0</v>
+      </c>
+      <c r="L16" s="83">
+        <f>J16-K16</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M16" s="82">
+        <v>0</v>
+      </c>
+      <c r="N16" s="82">
+        <v>0</v>
+      </c>
+      <c r="O16" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="76">
+        <f>17/100</f>
+        <v>0.17</v>
+      </c>
+      <c r="E17" s="60">
+        <v>11</v>
+      </c>
+      <c r="F17" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="3">
+      <c r="H17" s="81">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F17" s="55">
+      <c r="I17" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J17" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K17" s="82">
+        <v>0</v>
+      </c>
+      <c r="L17" s="83">
+        <f>J17-K17</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M17" s="82">
+        <v>0</v>
+      </c>
+      <c r="N17" s="82">
+        <v>0</v>
+      </c>
+      <c r="O17" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="78">
+        <v>0.16</v>
+      </c>
+      <c r="E18" s="60">
+        <v>10</v>
+      </c>
+      <c r="F18" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E18" s="3">
+      <c r="H18" s="81">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F18" s="55">
+      <c r="I18" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J18" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K18" s="82">
+        <v>0</v>
+      </c>
+      <c r="L18" s="83">
+        <f>J18-K18</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M18" s="82">
+        <v>0</v>
+      </c>
+      <c r="N18" s="82">
+        <v>0</v>
+      </c>
+      <c r="O18" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="78">
+        <v>0.16</v>
+      </c>
+      <c r="E19" s="60">
+        <v>9</v>
+      </c>
+      <c r="F19" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E19" s="3">
+      <c r="H19" s="81">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F19" s="55">
+      <c r="I19" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J19" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K19" s="82">
+        <v>0</v>
+      </c>
+      <c r="L19" s="83">
+        <f>J19-K19</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M19" s="82">
+        <v>0</v>
+      </c>
+      <c r="N19" s="82">
+        <v>0</v>
+      </c>
+      <c r="O19" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="78">
+        <v>0.16</v>
+      </c>
+      <c r="E20" s="60">
+        <v>8</v>
+      </c>
+      <c r="F20" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E20" s="3">
+      <c r="H20" s="81">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F20" s="55">
+      <c r="I20" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J20" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K20" s="82">
+        <v>0</v>
+      </c>
+      <c r="L20" s="83">
+        <f>J20-K20</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M20" s="82">
+        <v>0</v>
+      </c>
+      <c r="N20" s="82">
+        <v>0</v>
+      </c>
+      <c r="O20" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="80">
+        <v>0.16</v>
+      </c>
+      <c r="E21" s="60">
+        <v>7</v>
+      </c>
+      <c r="F21" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="3">
+      <c r="H21" s="81">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F21" s="55">
+      <c r="I21" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J21" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K21" s="82">
+        <v>0</v>
+      </c>
+      <c r="L21" s="83">
+        <f>J21-K21</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M21" s="82">
+        <v>0</v>
+      </c>
+      <c r="N21" s="82">
+        <v>0</v>
+      </c>
+      <c r="O21" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E22" s="60">
+        <v>6</v>
+      </c>
+      <c r="F22" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E22" s="3">
+      <c r="H22" s="81">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F22" s="55">
+      <c r="I22" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J22" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K22" s="82">
+        <v>0</v>
+      </c>
+      <c r="L22" s="83">
+        <f>J22-K22</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M22" s="82">
+        <v>0</v>
+      </c>
+      <c r="N22" s="82">
+        <v>0</v>
+      </c>
+      <c r="O22" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E23" s="60">
+        <v>5</v>
+      </c>
+      <c r="F23" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="3">
+      <c r="H23" s="81">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F23" s="55">
+      <c r="I23" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J23" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K23" s="82">
+        <v>0</v>
+      </c>
+      <c r="L23" s="83">
+        <f>J23-K23</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M23" s="82">
+        <v>0</v>
+      </c>
+      <c r="N23" s="82">
+        <v>0</v>
+      </c>
+      <c r="O23" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E24" s="60">
+        <v>4</v>
+      </c>
+      <c r="F24" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E24" s="3">
+      <c r="H24" s="81">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F24" s="55">
+      <c r="I24" s="81">
+        <f>$C$20</f>
+        <v>0.16</v>
+      </c>
+      <c r="J24" s="82">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K24" s="82">
+        <v>0</v>
+      </c>
+      <c r="L24" s="83">
+        <f>J24-K24</f>
+        <v>410.20299999999997</v>
+      </c>
+      <c r="M24" s="82">
+        <v>0</v>
+      </c>
+      <c r="N24" s="82">
+        <v>0</v>
+      </c>
+      <c r="O24" s="84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="73">
+        <f t="shared" si="2"/>
+        <v>199.76886100000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E25" s="60">
+        <v>3</v>
+      </c>
+      <c r="F25" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E25" s="3">
+      <c r="H25" s="58">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F25" s="55">
+      <c r="I25" s="58">
+        <f>C19</f>
+        <v>0.16</v>
+      </c>
+      <c r="J25" s="70">
+        <v>410.702</v>
+      </c>
+      <c r="K25" s="70">
+        <v>0</v>
+      </c>
+      <c r="L25" s="71">
+        <f>J25-K25</f>
+        <v>410.702</v>
+      </c>
+      <c r="M25" s="70">
+        <v>0</v>
+      </c>
+      <c r="N25" s="70">
+        <v>0</v>
+      </c>
+      <c r="O25" s="72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="73">
+        <f t="shared" si="2"/>
+        <v>200.01187400000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E26" s="60">
+        <v>2</v>
+      </c>
+      <c r="F26" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E26" s="3">
-        <v>3</v>
-      </c>
-      <c r="F26" s="55">
+      <c r="H26" s="58">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I26" s="58">
+        <f>C18</f>
+        <v>0.16</v>
+      </c>
+      <c r="J26" s="70">
+        <v>177.54900000000001</v>
+      </c>
+      <c r="K26" s="70">
+        <v>0</v>
+      </c>
+      <c r="L26" s="71">
+        <f>J26-K26</f>
+        <v>177.54900000000001</v>
+      </c>
+      <c r="M26" s="70">
+        <v>255.92599999999999</v>
+      </c>
+      <c r="N26" s="70">
+        <v>0</v>
+      </c>
+      <c r="O26" s="72">
+        <f t="shared" si="1"/>
+        <v>255.92599999999999</v>
+      </c>
+      <c r="P26" s="73">
+        <f t="shared" si="2"/>
+        <v>188.83676300000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E27" s="60">
+        <v>1</v>
+      </c>
+      <c r="F27" s="61">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E27" s="3">
-        <v>2</v>
-      </c>
-      <c r="F27" s="55">
+      <c r="H27" s="58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="58">
+        <f>C17</f>
+        <v>0.17</v>
+      </c>
+      <c r="J27" s="70">
+        <v>205.286</v>
+      </c>
+      <c r="K27" s="70">
+        <v>0</v>
+      </c>
+      <c r="L27" s="71">
+        <f t="shared" ref="L27:L28" si="3">J27-K27</f>
+        <v>205.286</v>
+      </c>
+      <c r="M27" s="70">
+        <v>514.17600000000004</v>
+      </c>
+      <c r="N27" s="70">
+        <v>0</v>
+      </c>
+      <c r="O27" s="72">
+        <f t="shared" si="1"/>
+        <v>514.17600000000004</v>
+      </c>
+      <c r="P27" s="73">
+        <f t="shared" si="2"/>
+        <v>323.63123200000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="66">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="67">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="55">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E29" s="3">
+      <c r="H28" s="69">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F29" s="55">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69">
+        <v>0</v>
+      </c>
+      <c r="L28" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69">
+        <v>0</v>
+      </c>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O29" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="P29" s="91">
+        <f>SUM(P4:P27)</f>
+        <v>4741.3130150000006</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O30" s="90"/>
+      <c r="P30" s="90"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O31" s="90"/>
+      <c r="P31" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1273,14 +2508,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A282A9DD-DDA8-407B-9F67-055CDE136535}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.109375" customWidth="1"/>
     <col min="6" max="6" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -1299,1495 +2534,1495 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>23</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>410.4</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <f>G3*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f>H3</f>
         <v>41.04</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <v>58.02</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="14">
         <v>53.12</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <v>0.2</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="16">
         <v>0.2</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="17">
         <f>J3*L3*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="13">
         <f>K3*M3*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="18">
         <f>I3/N3</f>
         <v>5.0524449697148754E-2</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3" s="19">
         <f>I3/O3</f>
         <v>5.5185025817555931E-2</v>
       </c>
-      <c r="R3" s="21" t="str">
+      <c r="R3" s="20" t="str">
         <f>IF(OR(N3&lt;I3,O3&lt;I3),"MALO","WENO")</f>
         <v>WENO</v>
       </c>
-      <c r="T3" s="22">
+      <c r="T3" s="21">
         <f>N3-I3</f>
         <v>771.24000000000024</v>
       </c>
-      <c r="U3" s="23">
+      <c r="U3" s="22">
         <f>O3-I3</f>
         <v>702.6400000000001</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="49">
         <v>0.1</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>22</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>410.4</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <f>G4*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f>I3+H4</f>
         <v>82.08</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>58.02</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="14">
         <v>53.12</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="15">
         <v>0.2</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>0.2</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <f>J4*L4*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="13">
         <f>K4*M4*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="18">
         <f t="shared" ref="P4:P26" si="0">I4/N4</f>
         <v>0.10104889939429751</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="19">
         <f t="shared" ref="Q4:Q26" si="1">I4/O4</f>
         <v>0.11037005163511186</v>
       </c>
-      <c r="R4" s="21" t="str">
+      <c r="R4" s="20" t="str">
         <f t="shared" ref="R4:R26" si="2">IF(OR(N4&lt;I4,O4&lt;I4),"MALO","WENO")</f>
         <v>WENO</v>
       </c>
-      <c r="T4" s="24">
+      <c r="T4" s="23">
         <f t="shared" ref="T4:T26" si="3">N4-I4</f>
         <v>730.20000000000016</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="24">
         <f t="shared" ref="U4:U26" si="4">O4-I4</f>
         <v>661.6</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>7</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>21</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>410.4</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <f>G5*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" ref="I5:I26" si="5">I4+H5</f>
         <v>123.12</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>58.02</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="14">
         <v>53.12</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>0.2</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="16">
         <v>0.2</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <f>J5*L5*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="13">
         <f>K5*M5*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="18">
         <f t="shared" si="0"/>
         <v>0.15157334909144626</v>
       </c>
-      <c r="Q5" s="20">
+      <c r="Q5" s="19">
         <f t="shared" si="1"/>
         <v>0.16555507745266781</v>
       </c>
-      <c r="R5" s="21" t="str">
+      <c r="R5" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T5" s="24">
+      <c r="T5" s="23">
         <f t="shared" si="3"/>
         <v>689.1600000000002</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5" s="24">
         <f t="shared" si="4"/>
         <v>620.56000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f>D5/1000</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="11">
+      <c r="E6" s="25"/>
+      <c r="F6" s="10">
         <v>20</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>410.4</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <f>G6*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" si="5"/>
         <v>164.16</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>58.02</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <v>53.12</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="15">
         <v>0.2</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <v>0.2</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="17">
         <f>J6*L6*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f>K6*M6*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="18">
         <f t="shared" si="0"/>
         <v>0.20209779878859502</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="19">
         <f t="shared" si="1"/>
         <v>0.22074010327022373</v>
       </c>
-      <c r="R6" s="21" t="str">
+      <c r="R6" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="23">
         <f t="shared" si="3"/>
         <v>648.12000000000023</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6" s="24">
         <f t="shared" si="4"/>
         <v>579.5200000000001</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>19</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>410.4</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <f>G7*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" si="5"/>
         <v>205.2</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>58.02</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="14">
         <v>53.12</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="15">
         <v>0.2</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>0.2</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="17">
         <f>J7*L7*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <f>K7*M7*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="18">
         <f t="shared" si="0"/>
         <v>0.25262224848574377</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="19">
         <f t="shared" si="1"/>
         <v>0.27592512908777966</v>
       </c>
-      <c r="R7" s="21" t="str">
+      <c r="R7" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T7" s="24">
+      <c r="T7" s="23">
         <f t="shared" si="3"/>
         <v>607.08000000000015</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="24">
         <f t="shared" si="4"/>
         <v>538.48</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="F8" s="11">
+      <c r="A8" s="26"/>
+      <c r="F8" s="10">
         <v>18</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>410.4</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <f>G8*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <f t="shared" si="5"/>
         <v>246.23999999999998</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <v>58.02</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="14">
         <v>53.12</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="15">
         <v>0.2</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>0.2</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <f>J8*L8*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <f>K8*M8*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="18">
         <f t="shared" si="0"/>
         <v>0.30314669818289253</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="19">
         <f t="shared" si="1"/>
         <v>0.33111015490533557</v>
       </c>
-      <c r="R8" s="21" t="str">
+      <c r="R8" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T8" s="24">
+      <c r="T8" s="23">
         <f t="shared" si="3"/>
         <v>566.04000000000019</v>
       </c>
-      <c r="U8" s="25">
+      <c r="U8" s="24">
         <f t="shared" si="4"/>
         <v>497.44000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="27"/>
-      <c r="F9" s="11">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="26"/>
+      <c r="F9" s="10">
         <v>17</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>410.4</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <f>G9*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <f t="shared" si="5"/>
         <v>287.27999999999997</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <v>58.02</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="14">
         <v>53.12</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="15">
         <v>0.2</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="16">
         <v>0.2</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="17">
         <f>J9*L9*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="13">
         <f>K9*M9*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="18">
         <f t="shared" si="0"/>
         <v>0.35367114788004123</v>
       </c>
-      <c r="Q9" s="20">
+      <c r="Q9" s="19">
         <f t="shared" si="1"/>
         <v>0.38629518072289148</v>
       </c>
-      <c r="R9" s="21" t="str">
+      <c r="R9" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T9" s="24">
+      <c r="T9" s="23">
         <f t="shared" si="3"/>
         <v>525.00000000000023</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9" s="24">
         <f t="shared" si="4"/>
         <v>456.40000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27"/>
-      <c r="F10" s="11">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="26"/>
+      <c r="F10" s="10">
         <v>16</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>410.4</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <f>G10*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <f t="shared" si="5"/>
         <v>328.32</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <v>58.02</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="14">
         <v>53.12</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="15">
         <v>0.2</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <v>0.2</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="17">
         <f>J10*L10*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="13">
         <f>K10*M10*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="18">
         <f t="shared" si="0"/>
         <v>0.40419559757719004</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="19">
         <f t="shared" si="1"/>
         <v>0.44148020654044745</v>
       </c>
-      <c r="R10" s="21" t="str">
+      <c r="R10" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T10" s="24">
+      <c r="T10" s="23">
         <f t="shared" si="3"/>
         <v>483.96000000000021</v>
       </c>
-      <c r="U10" s="25">
+      <c r="U10" s="24">
         <f t="shared" si="4"/>
         <v>415.36000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="F11" s="11">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="F11" s="10">
         <v>15</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>410.4</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <f>G11*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <f t="shared" si="5"/>
         <v>369.36</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <v>58.02</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="14">
         <v>53.12</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>0.2</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="16">
         <v>0.2</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <f>J11*L11*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="13">
         <f>K11*M11*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="18">
         <f t="shared" si="0"/>
         <v>0.45472004727433879</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="19">
         <f t="shared" si="1"/>
         <v>0.49666523235800342</v>
       </c>
-      <c r="R11" s="21" t="str">
+      <c r="R11" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T11" s="24">
+      <c r="T11" s="23">
         <f t="shared" si="3"/>
         <v>442.92000000000019</v>
       </c>
-      <c r="U11" s="25">
+      <c r="U11" s="24">
         <f t="shared" si="4"/>
         <v>374.32000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="27"/>
-      <c r="F12" s="11">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="26"/>
+      <c r="F12" s="10">
         <v>14</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>410.4</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f>G12*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <f t="shared" si="5"/>
         <v>410.40000000000003</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <v>58.02</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="14">
         <v>53.12</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="15">
         <v>0.2</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <v>0.2</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <f>J12*L12*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="13">
         <f>K12*M12*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="18">
         <f t="shared" si="0"/>
         <v>0.50524449697148754</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="19">
         <f t="shared" si="1"/>
         <v>0.55185025817555933</v>
       </c>
-      <c r="R12" s="21" t="str">
+      <c r="R12" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T12" s="24">
+      <c r="T12" s="23">
         <f t="shared" si="3"/>
         <v>401.88000000000017</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="24">
         <f t="shared" si="4"/>
         <v>333.28000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="27"/>
-      <c r="F13" s="11">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="26"/>
+      <c r="F13" s="10">
         <v>13</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="11">
         <v>410.4</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <f>G13*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="12">
         <f t="shared" si="5"/>
         <v>451.44000000000005</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <v>58.02</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="14">
         <v>53.12</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="15">
         <v>0.2</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="16">
         <v>0.2</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="17">
         <f>J13*L13*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="13">
         <f>K13*M13*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="18">
         <f t="shared" si="0"/>
         <v>0.55576894666863641</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="19">
         <f t="shared" si="1"/>
         <v>0.60703528399311535</v>
       </c>
-      <c r="R13" s="21" t="str">
+      <c r="R13" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T13" s="24">
+      <c r="T13" s="23">
         <f t="shared" si="3"/>
         <v>360.84000000000015</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13" s="24">
         <f t="shared" si="4"/>
         <v>292.24</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="F14" s="11">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="26"/>
+      <c r="F14" s="10">
         <v>12</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <v>410.4</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <f>G14*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="12">
         <f t="shared" si="5"/>
         <v>492.48000000000008</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <v>58.02</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="14">
         <v>53.12</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="15">
         <v>0.2</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="16">
         <v>0.2</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="17">
         <f>J14*L14*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="13">
         <f>K14*M14*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="18">
         <f t="shared" si="0"/>
         <v>0.60629339636578516</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="19">
         <f t="shared" si="1"/>
         <v>0.66222030981067126</v>
       </c>
-      <c r="R14" s="21" t="str">
+      <c r="R14" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T14" s="24">
+      <c r="T14" s="23">
         <f t="shared" si="3"/>
         <v>319.80000000000013</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="24">
         <f t="shared" si="4"/>
         <v>251.2</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="27"/>
-      <c r="F15" s="11">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="26"/>
+      <c r="F15" s="10">
         <v>11</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="11">
         <v>410.4</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <f>G15*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="12">
         <f t="shared" si="5"/>
         <v>533.5200000000001</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <v>58.02</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="14">
         <v>53.12</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="15">
         <v>0.2</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="16">
         <v>0.2</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="17">
         <f>J15*L15*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="13">
         <f>K15*M15*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="18">
         <f t="shared" si="0"/>
         <v>0.65681784606293392</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="19">
         <f t="shared" si="1"/>
         <v>0.71740533562822728</v>
       </c>
-      <c r="R15" s="21" t="str">
+      <c r="R15" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T15" s="24">
+      <c r="T15" s="23">
         <f t="shared" si="3"/>
         <v>278.7600000000001</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="24">
         <f t="shared" si="4"/>
         <v>210.15999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="27"/>
-      <c r="F16" s="11">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="F16" s="10">
         <v>10</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <v>410.4</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <f>G16*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="12">
         <f t="shared" si="5"/>
         <v>574.56000000000006</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <v>58.02</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="14">
         <v>53.12</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="15">
         <v>0.2</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="16">
         <v>0.2</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="17">
         <f>J16*L16*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16" s="13">
         <f>K16*M16*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <f t="shared" si="0"/>
         <v>0.70734229576008267</v>
       </c>
-      <c r="Q16" s="20">
+      <c r="Q16" s="19">
         <f t="shared" si="1"/>
         <v>0.77259036144578319</v>
       </c>
-      <c r="R16" s="21" t="str">
+      <c r="R16" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T16" s="24">
+      <c r="T16" s="23">
         <f t="shared" si="3"/>
         <v>237.72000000000014</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="24">
         <f t="shared" si="4"/>
         <v>169.12</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="27"/>
-      <c r="F17" s="11">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="26"/>
+      <c r="F17" s="10">
         <v>9</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <v>410.4</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <f>G17*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="12">
         <f t="shared" si="5"/>
         <v>615.6</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <v>58.02</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="14">
         <v>53.12</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="15">
         <v>0.2</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="16">
         <v>0.2</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="17">
         <f>J17*L17*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17" s="13">
         <f>K17*M17*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="18">
         <f t="shared" si="0"/>
         <v>0.75786674545723132</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="19">
         <f t="shared" si="1"/>
         <v>0.82777538726333899</v>
       </c>
-      <c r="R17" s="21" t="str">
+      <c r="R17" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T17" s="24">
+      <c r="T17" s="23">
         <f t="shared" si="3"/>
         <v>196.68000000000018</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17" s="24">
         <f t="shared" si="4"/>
         <v>128.08000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="27"/>
-      <c r="F18" s="11">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="26"/>
+      <c r="F18" s="10">
         <v>8</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="11">
         <v>410.4</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <f>G18*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="12">
         <f t="shared" si="5"/>
         <v>656.64</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <v>58.02</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="14">
         <v>53.12</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="15">
         <v>0.2</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="16">
         <v>0.2</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="17">
         <f>J18*L18*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O18" s="14">
+      <c r="O18" s="13">
         <f>K18*M18*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="18">
         <f t="shared" si="0"/>
         <v>0.80839119515438007</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <f t="shared" si="1"/>
         <v>0.8829604130808949</v>
       </c>
-      <c r="R18" s="21" t="str">
+      <c r="R18" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T18" s="24">
+      <c r="T18" s="23">
         <f t="shared" si="3"/>
         <v>155.64000000000021</v>
       </c>
-      <c r="U18" s="25">
+      <c r="U18" s="24">
         <f t="shared" si="4"/>
         <v>87.040000000000077</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="27"/>
-      <c r="F19" s="11">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="26"/>
+      <c r="F19" s="10">
         <v>7</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11">
         <v>410.4</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="11">
         <f>G19*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="12">
         <f t="shared" si="5"/>
         <v>697.68</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <v>58.02</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="14">
         <v>53.12</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="15">
         <v>0.2</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="16">
         <v>0.2</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="17">
         <f>J19*L19*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="13">
         <f>K19*M19*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="18">
         <f t="shared" si="0"/>
         <v>0.85891564485152871</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <f t="shared" si="1"/>
         <v>0.93814543889845081</v>
       </c>
-      <c r="R19" s="21" t="str">
+      <c r="R19" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T19" s="24">
+      <c r="T19" s="23">
         <f t="shared" si="3"/>
         <v>114.60000000000025</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="24">
         <f t="shared" si="4"/>
         <v>46.000000000000114</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="F20" s="11">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="F20" s="10">
         <v>6</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="11">
         <v>410.4</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="11">
         <f>G20*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="12">
         <f t="shared" si="5"/>
         <v>738.71999999999991</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <v>58.02</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="14">
         <v>53.12</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L20" s="15">
         <v>0.2</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="16">
         <v>0.2</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="17">
         <f>J20*L20*$D$6*100*100</f>
         <v>812.2800000000002</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20" s="13">
         <f>K20*M20*$D$6*100*100</f>
         <v>743.68000000000006</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="18">
         <f t="shared" si="0"/>
         <v>0.90944009454867747</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q20" s="19">
         <f t="shared" si="1"/>
         <v>0.99333046471600672</v>
       </c>
-      <c r="R20" s="21" t="str">
+      <c r="R20" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T20" s="24">
+      <c r="T20" s="23">
         <f t="shared" si="3"/>
         <v>73.560000000000286</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20" s="24">
         <f t="shared" si="4"/>
         <v>4.9600000000001501</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="27"/>
-      <c r="F21" s="11">
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="26"/>
+      <c r="F21" s="10">
         <v>5</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="11">
         <v>410.4</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="11">
         <f>G21*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <f t="shared" si="5"/>
         <v>779.75999999999988</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <v>58.02</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="14">
         <v>53.12</v>
       </c>
-      <c r="L21" s="30">
+      <c r="L21" s="29">
         <v>0.25</v>
       </c>
-      <c r="M21" s="31">
+      <c r="M21" s="30">
         <v>0.25</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="17">
         <f>J21*L21*$D$6*100*100</f>
         <v>1015.3500000000001</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="13">
         <f>K21*M21*$D$6*100*100</f>
         <v>929.59999999999991</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="18">
         <f t="shared" si="0"/>
         <v>0.76797163539666102</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="19">
         <f t="shared" si="1"/>
         <v>0.83881239242685024</v>
       </c>
-      <c r="R21" s="21" t="str">
+      <c r="R21" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T21" s="24">
+      <c r="T21" s="23">
         <f t="shared" si="3"/>
         <v>235.59000000000026</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="24">
         <f t="shared" si="4"/>
         <v>149.84000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>4</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11">
         <v>410.4</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <f>G22*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <f t="shared" si="5"/>
         <v>820.79999999999984</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="13">
         <v>58.02</v>
       </c>
-      <c r="K22" s="15">
+      <c r="K22" s="14">
         <v>53.12</v>
       </c>
-      <c r="L22" s="30">
+      <c r="L22" s="29">
         <v>0.25</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="30">
         <v>0.25</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="17">
         <f>J22*L22*$D$6*100*100</f>
         <v>1015.3500000000001</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22" s="13">
         <f>K22*M22*$D$6*100*100</f>
         <v>929.59999999999991</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="18">
         <f t="shared" si="0"/>
         <v>0.80839119515437996</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="19">
         <f t="shared" si="1"/>
         <v>0.8829604130808949</v>
       </c>
-      <c r="R22" s="21" t="str">
+      <c r="R22" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T22" s="24">
+      <c r="T22" s="23">
         <f t="shared" si="3"/>
         <v>194.5500000000003</v>
       </c>
-      <c r="U22" s="25">
+      <c r="U22" s="24">
         <f t="shared" si="4"/>
         <v>108.80000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>3</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <v>410.4</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <f>G23*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="12">
         <f t="shared" si="5"/>
         <v>861.8399999999998</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="13">
         <v>58.02</v>
       </c>
-      <c r="K23" s="15">
+      <c r="K23" s="14">
         <v>50.03</v>
       </c>
-      <c r="L23" s="30">
+      <c r="L23" s="29">
         <v>0.25</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="30">
         <v>0.25</v>
       </c>
-      <c r="N23" s="18">
+      <c r="N23" s="17">
         <f>J23*L23*$D$6*100*100</f>
         <v>1015.3500000000001</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23" s="13">
         <f>K23*M23*$D$6*100*100</f>
         <v>875.52499999999998</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="18">
         <f t="shared" si="0"/>
         <v>0.84881075491209901</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="19">
         <f t="shared" si="1"/>
         <v>0.984369378372976</v>
       </c>
-      <c r="R23" s="21" t="str">
+      <c r="R23" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T23" s="24">
+      <c r="T23" s="23">
         <f t="shared" si="3"/>
         <v>153.51000000000033</v>
       </c>
-      <c r="U23" s="25">
+      <c r="U23" s="24">
         <f t="shared" si="4"/>
         <v>13.685000000000173</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
-      <c r="F24" s="11">
+      <c r="C24" s="4"/>
+      <c r="F24" s="10">
         <v>2</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="11">
         <v>410.4</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="31">
         <f>G24*$D$3*$D$4</f>
         <v>41.04</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <f t="shared" si="5"/>
         <v>902.87999999999977</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="13">
         <v>57.05</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="14">
         <v>45</v>
       </c>
-      <c r="L24" s="33">
+      <c r="L24" s="32">
         <v>0.25</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="33">
         <v>0.3</v>
       </c>
-      <c r="N24" s="18">
+      <c r="N24" s="17">
         <f>J24*L24*$D$6*100*100</f>
         <v>998.37499999999989</v>
       </c>
-      <c r="O24" s="14">
+      <c r="O24" s="13">
         <f>K24*M24*$D$6*100*100</f>
         <v>944.99999999999989</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="18">
         <f t="shared" si="0"/>
         <v>0.90434956804807798</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="19">
         <f t="shared" si="1"/>
         <v>0.95542857142857129</v>
       </c>
-      <c r="R24" s="21" t="str">
+      <c r="R24" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T24" s="24">
+      <c r="T24" s="23">
         <f t="shared" si="3"/>
         <v>95.495000000000118</v>
       </c>
-      <c r="U24" s="25">
+      <c r="U24" s="24">
         <f t="shared" si="4"/>
         <v>42.120000000000118</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <v>1</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="11">
         <v>467.16049999999996</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="31">
         <f>G25*$D$3*$D$4</f>
         <v>46.716049999999996</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I25" s="34">
         <f t="shared" si="5"/>
         <v>949.59604999999976</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="13">
         <v>67.650000000000006</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="14">
         <v>48.88</v>
       </c>
-      <c r="L25" s="33">
+      <c r="L25" s="32">
         <v>0.25</v>
       </c>
-      <c r="M25" s="34">
+      <c r="M25" s="33">
         <v>0.3</v>
       </c>
-      <c r="N25" s="18">
+      <c r="N25" s="17">
         <f>J25*L25*$D$6*100*100</f>
         <v>1183.875</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25" s="13">
         <f>K25*M25*$D$6*100*100</f>
         <v>1026.48</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P25" s="18">
         <f t="shared" si="0"/>
         <v>0.80210837292788495</v>
       </c>
-      <c r="Q25" s="20">
+      <c r="Q25" s="19">
         <f t="shared" si="1"/>
         <v>0.92509941742654489</v>
       </c>
-      <c r="R25" s="21" t="str">
+      <c r="R25" s="20" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T25" s="24">
+      <c r="T25" s="23">
         <f t="shared" si="3"/>
         <v>234.27895000000024</v>
       </c>
-      <c r="U25" s="25">
+      <c r="U25" s="24">
         <f t="shared" si="4"/>
         <v>76.883950000000254</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="36">
+      <c r="F26" s="35">
         <v>-1</v>
       </c>
-      <c r="G26" s="49">
+      <c r="G26" s="48">
         <v>734.65999999999985</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="36">
         <f>G26*$D$3*$D$4</f>
         <v>73.465999999999994</v>
       </c>
-      <c r="I26" s="38">
+      <c r="I26" s="37">
         <f t="shared" si="5"/>
         <v>1023.0620499999998</v>
       </c>
-      <c r="J26" s="39">
+      <c r="J26" s="38">
         <v>84.59</v>
       </c>
-      <c r="K26" s="40">
+      <c r="K26" s="39">
         <v>50.55</v>
       </c>
-      <c r="L26" s="41">
+      <c r="L26" s="40">
         <v>0.25</v>
       </c>
-      <c r="M26" s="42">
+      <c r="M26" s="41">
         <v>0.3</v>
       </c>
-      <c r="N26" s="43">
+      <c r="N26" s="42">
         <f>J26*L26*$D$6*100*100</f>
         <v>1480.3250000000003</v>
       </c>
-      <c r="O26" s="39">
+      <c r="O26" s="38">
         <f>K26*M26*$D$6*100*100</f>
         <v>1061.5500000000002</v>
       </c>
-      <c r="P26" s="44">
+      <c r="P26" s="43">
         <f t="shared" si="0"/>
         <v>0.69110637866684654</v>
       </c>
-      <c r="Q26" s="45">
+      <c r="Q26" s="44">
         <f t="shared" si="1"/>
         <v>0.96374362959822868</v>
       </c>
-      <c r="R26" s="46" t="str">
+      <c r="R26" s="45" t="str">
         <f t="shared" si="2"/>
         <v>WENO</v>
       </c>
-      <c r="T26" s="47">
+      <c r="T26" s="46">
         <f t="shared" si="3"/>
         <v>457.2629500000005</v>
       </c>
-      <c r="U26" s="48">
+      <c r="U26" s="47">
         <f t="shared" si="4"/>
         <v>38.48795000000041</v>
       </c>

</xml_diff>

<commit_message>
Corrige área losa multiplicada por enlucido
</commit_message>
<xml_diff>
--- a/Tarea 03/Cubicaciones.xlsx
+++ b/Tarea 03/Cubicaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F56E787A-D088-43BE-9D78-923704147FA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5C336B50-61B8-4BD8-A579-363ADB3AE927}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Estuco</t>
   </si>
@@ -280,9 +280,6 @@
     <t>[T/cm^2]</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>Alosa</t>
   </si>
   <si>
@@ -322,9 +319,6 @@
     <t>Área losa interior final (m2)</t>
   </si>
   <si>
-    <t>Área losa estacionamiento final (m2)</t>
-  </si>
-  <si>
     <t>Peso total (T)</t>
   </si>
   <si>
@@ -349,7 +343,7 @@
     <t>Espesor losas</t>
   </si>
   <si>
-    <t>$\gamma_{Eslucido}$</t>
+    <t>$\gamma_{Enlucido}$</t>
   </si>
 </sst>
 </file>
@@ -410,7 +404,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,12 +449,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -759,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -975,9 +963,6 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1011,19 +996,13 @@
     <xf numFmtId="2" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1324,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P31"/>
+  <dimension ref="B2:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,25 +1323,23 @@
     <col min="11" max="11" width="11.77734375" style="52" customWidth="1"/>
     <col min="12" max="12" width="11.21875" style="52" customWidth="1"/>
     <col min="13" max="13" width="15.5546875" style="52" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" style="52" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" style="52" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" style="52" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="52"/>
+    <col min="14" max="14" width="9.6640625" style="52" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="52"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="50" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="51"/>
     </row>
-    <row r="3" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="53" t="s">
         <v>6</v>
       </c>
@@ -1370,40 +1347,34 @@
         <v>3</v>
       </c>
       <c r="E3" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="87" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="87" t="s">
+      <c r="H3" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="M3" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="86" t="s">
+      <c r="N3" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="85" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="89" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="56" t="s">
         <v>2</v>
       </c>
@@ -1437,19 +1408,12 @@
       <c r="M4" s="70">
         <v>0</v>
       </c>
-      <c r="N4" s="70">
-        <v>0</v>
-      </c>
-      <c r="O4" s="72">
-        <f>M4-N4</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="73">
-        <f>L4*($C$4*I4+$C$6*$C$12+$C$7*$C$13)+I4*O4*$C$4</f>
+      <c r="N4" s="72">
+        <f>I4*J4*$C$4+L4*($C$6*$C$12+$C$7*$C$13)+I4*M4*$C$4</f>
         <v>33.455925999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="60" t="s">
         <v>5</v>
       </c>
@@ -1462,40 +1426,33 @@
       <c r="F5" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H5" s="81">
+      <c r="H5" s="80">
         <f t="shared" ref="H5:H28" si="0">E5</f>
         <v>23</v>
       </c>
-      <c r="I5" s="81">
+      <c r="I5" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J5" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K5" s="82">
-        <v>0</v>
-      </c>
-      <c r="L5" s="83">
+      <c r="J5" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K5" s="81">
+        <v>0</v>
+      </c>
+      <c r="L5" s="82">
         <f>J5-K5</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M5" s="82">
-        <v>0</v>
-      </c>
-      <c r="N5" s="82">
-        <v>0</v>
-      </c>
-      <c r="O5" s="84">
-        <f t="shared" ref="O5:O27" si="1">M5-N5</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="73">
-        <f t="shared" ref="P5:P27" si="2">L5*($C$4*I5+$C$6*$C$12+$C$7*$C$13)+I5*O5*$C$4</f>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M5" s="81">
+        <v>0</v>
+      </c>
+      <c r="N5" s="83">
+        <f t="shared" ref="N5:N27" si="1">I5*J5*$C$4+L5*($C$6*$C$12+$C$7*$C$13)+I5*M5*$C$4</f>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="60" t="s">
         <v>4</v>
       </c>
@@ -1508,42 +1465,35 @@
       <c r="F6" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H6" s="81">
+      <c r="H6" s="80">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="I6" s="81">
+      <c r="I6" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J6" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K6" s="82">
-        <v>0</v>
-      </c>
-      <c r="L6" s="83">
+      <c r="J6" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K6" s="81">
+        <v>0</v>
+      </c>
+      <c r="L6" s="82">
         <f>J6-K6</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M6" s="82">
-        <v>0</v>
-      </c>
-      <c r="N6" s="82">
-        <v>0</v>
-      </c>
-      <c r="O6" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="81">
+        <v>0</v>
+      </c>
+      <c r="N6" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="62">
         <v>0.4</v>
@@ -1554,82 +1504,68 @@
       <c r="F7" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H7" s="81">
+      <c r="H7" s="80">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="I7" s="81">
+      <c r="I7" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J7" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K7" s="82">
-        <v>0</v>
-      </c>
-      <c r="L7" s="83">
+      <c r="J7" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K7" s="81">
+        <v>0</v>
+      </c>
+      <c r="L7" s="82">
         <f>J7-K7</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M7" s="82">
-        <v>0</v>
-      </c>
-      <c r="N7" s="82">
-        <v>0</v>
-      </c>
-      <c r="O7" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M7" s="81">
+        <v>0</v>
+      </c>
+      <c r="N7" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E8" s="60">
         <v>20</v>
       </c>
       <c r="F8" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H8" s="81">
+      <c r="H8" s="80">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I8" s="81">
+      <c r="I8" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J8" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K8" s="82">
-        <v>0</v>
-      </c>
-      <c r="L8" s="83">
+      <c r="J8" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K8" s="81">
+        <v>0</v>
+      </c>
+      <c r="L8" s="82">
         <f>J8-K8</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M8" s="82">
-        <v>0</v>
-      </c>
-      <c r="N8" s="82">
-        <v>0</v>
-      </c>
-      <c r="O8" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M8" s="81">
+        <v>0</v>
+      </c>
+      <c r="N8" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="60">
         <v>19</v>
@@ -1637,45 +1573,38 @@
       <c r="F9" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H9" s="81">
+      <c r="H9" s="80">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="I9" s="81">
+      <c r="I9" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J9" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K9" s="82">
-        <v>0</v>
-      </c>
-      <c r="L9" s="83">
+      <c r="J9" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K9" s="81">
+        <v>0</v>
+      </c>
+      <c r="L9" s="82">
         <f>J9-K9</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M9" s="82">
-        <v>0</v>
-      </c>
-      <c r="N9" s="82">
-        <v>0</v>
-      </c>
-      <c r="O9" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M9" s="81">
+        <v>0</v>
+      </c>
+      <c r="N9" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="63" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="60">
         <v>18</v>
@@ -1683,40 +1612,33 @@
       <c r="F10" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H10" s="81">
+      <c r="H10" s="80">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I10" s="81">
+      <c r="I10" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J10" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K10" s="82">
-        <v>0</v>
-      </c>
-      <c r="L10" s="83">
+      <c r="J10" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K10" s="81">
+        <v>0</v>
+      </c>
+      <c r="L10" s="82">
         <f>J10-K10</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M10" s="82">
-        <v>0</v>
-      </c>
-      <c r="N10" s="82">
-        <v>0</v>
-      </c>
-      <c r="O10" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M10" s="81">
+        <v>0</v>
+      </c>
+      <c r="N10" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="64" t="s">
         <v>0</v>
       </c>
@@ -1730,40 +1652,33 @@
       <c r="F11" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H11" s="81">
+      <c r="H11" s="80">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="I11" s="81">
+      <c r="I11" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J11" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K11" s="82">
-        <v>0</v>
-      </c>
-      <c r="L11" s="83">
+      <c r="J11" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K11" s="81">
+        <v>0</v>
+      </c>
+      <c r="L11" s="82">
         <f>J11-K11</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M11" s="82">
-        <v>0</v>
-      </c>
-      <c r="N11" s="82">
-        <v>0</v>
-      </c>
-      <c r="O11" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M11" s="81">
+        <v>0</v>
+      </c>
+      <c r="N11" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="65" t="s">
         <v>1</v>
       </c>
@@ -1777,42 +1692,35 @@
       <c r="F12" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H12" s="81">
+      <c r="H12" s="80">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I12" s="81">
+      <c r="I12" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J12" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K12" s="82">
-        <v>0</v>
-      </c>
-      <c r="L12" s="83">
+      <c r="J12" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K12" s="81">
+        <v>0</v>
+      </c>
+      <c r="L12" s="82">
         <f>J12-K12</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M12" s="82">
-        <v>0</v>
-      </c>
-      <c r="N12" s="82">
-        <v>0</v>
-      </c>
-      <c r="O12" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M12" s="81">
+        <v>0</v>
+      </c>
+      <c r="N12" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="66" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="62">
         <v>0.03</v>
@@ -1823,125 +1731,104 @@
       <c r="F13" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H13" s="81">
+      <c r="H13" s="80">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I13" s="81">
+      <c r="I13" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J13" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K13" s="82">
-        <v>0</v>
-      </c>
-      <c r="L13" s="83">
+      <c r="J13" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K13" s="81">
+        <v>0</v>
+      </c>
+      <c r="L13" s="82">
         <f>J13-K13</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M13" s="82">
-        <v>0</v>
-      </c>
-      <c r="N13" s="82">
-        <v>0</v>
-      </c>
-      <c r="O13" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M13" s="81">
+        <v>0</v>
+      </c>
+      <c r="N13" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E14" s="60">
         <v>14</v>
       </c>
       <c r="F14" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H14" s="81">
+      <c r="H14" s="80">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I14" s="81">
+      <c r="I14" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J14" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K14" s="82">
-        <v>0</v>
-      </c>
-      <c r="L14" s="83">
+      <c r="J14" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K14" s="81">
+        <v>0</v>
+      </c>
+      <c r="L14" s="82">
         <f>J14-K14</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M14" s="82">
-        <v>0</v>
-      </c>
-      <c r="N14" s="82">
-        <v>0</v>
-      </c>
-      <c r="O14" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="51" t="s">
-        <v>53</v>
-      </c>
+      <c r="M14" s="81">
+        <v>0</v>
+      </c>
+      <c r="N14" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E15" s="60">
         <v>13</v>
       </c>
       <c r="F15" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H15" s="81">
+      <c r="H15" s="80">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="I15" s="81">
+      <c r="I15" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J15" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K15" s="82">
-        <v>0</v>
-      </c>
-      <c r="L15" s="83">
+      <c r="J15" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K15" s="81">
+        <v>0</v>
+      </c>
+      <c r="L15" s="82">
         <f>J15-K15</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M15" s="82">
-        <v>0</v>
-      </c>
-      <c r="N15" s="82">
-        <v>0</v>
-      </c>
-      <c r="O15" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="74" t="s">
-        <v>47</v>
+      <c r="M15" s="81">
+        <v>0</v>
+      </c>
+      <c r="N15" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>45</v>
       </c>
       <c r="E16" s="60">
         <v>12</v>
@@ -1949,44 +1836,37 @@
       <c r="F16" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H16" s="81">
+      <c r="H16" s="80">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I16" s="81">
+      <c r="I16" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J16" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K16" s="82">
-        <v>0</v>
-      </c>
-      <c r="L16" s="83">
+      <c r="J16" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K16" s="81">
+        <v>0</v>
+      </c>
+      <c r="L16" s="82">
         <f>J16-K16</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M16" s="82">
-        <v>0</v>
-      </c>
-      <c r="N16" s="82">
-        <v>0</v>
-      </c>
-      <c r="O16" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="76">
+      <c r="M16" s="81">
+        <v>0</v>
+      </c>
+      <c r="N16" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="75">
         <f>17/100</f>
         <v>0.17</v>
       </c>
@@ -1996,44 +1876,37 @@
       <c r="F17" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H17" s="81">
+      <c r="H17" s="80">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="I17" s="81">
+      <c r="I17" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J17" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K17" s="82">
-        <v>0</v>
-      </c>
-      <c r="L17" s="83">
+      <c r="J17" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K17" s="81">
+        <v>0</v>
+      </c>
+      <c r="L17" s="82">
         <f>J17-K17</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M17" s="82">
-        <v>0</v>
-      </c>
-      <c r="N17" s="82">
-        <v>0</v>
-      </c>
-      <c r="O17" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="78">
+      <c r="M17" s="81">
+        <v>0</v>
+      </c>
+      <c r="N17" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="77">
         <v>0.16</v>
       </c>
       <c r="E18" s="60">
@@ -2042,44 +1915,37 @@
       <c r="F18" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H18" s="81">
+      <c r="H18" s="80">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I18" s="81">
+      <c r="I18" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J18" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K18" s="82">
-        <v>0</v>
-      </c>
-      <c r="L18" s="83">
+      <c r="J18" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K18" s="81">
+        <v>0</v>
+      </c>
+      <c r="L18" s="82">
         <f>J18-K18</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M18" s="82">
-        <v>0</v>
-      </c>
-      <c r="N18" s="82">
-        <v>0</v>
-      </c>
-      <c r="O18" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="78">
+      <c r="M18" s="81">
+        <v>0</v>
+      </c>
+      <c r="N18" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="77">
         <v>0.16</v>
       </c>
       <c r="E19" s="60">
@@ -2088,44 +1954,37 @@
       <c r="F19" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H19" s="81">
+      <c r="H19" s="80">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I19" s="81">
+      <c r="I19" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J19" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K19" s="82">
-        <v>0</v>
-      </c>
-      <c r="L19" s="83">
+      <c r="J19" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K19" s="81">
+        <v>0</v>
+      </c>
+      <c r="L19" s="82">
         <f>J19-K19</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M19" s="82">
-        <v>0</v>
-      </c>
-      <c r="N19" s="82">
-        <v>0</v>
-      </c>
-      <c r="O19" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="78">
+      <c r="M19" s="81">
+        <v>0</v>
+      </c>
+      <c r="N19" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="77">
         <v>0.16</v>
       </c>
       <c r="E20" s="60">
@@ -2134,44 +1993,37 @@
       <c r="F20" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H20" s="81">
+      <c r="H20" s="80">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I20" s="81">
+      <c r="I20" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J20" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K20" s="82">
-        <v>0</v>
-      </c>
-      <c r="L20" s="83">
+      <c r="J20" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K20" s="81">
+        <v>0</v>
+      </c>
+      <c r="L20" s="82">
         <f>J20-K20</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M20" s="82">
-        <v>0</v>
-      </c>
-      <c r="N20" s="82">
-        <v>0</v>
-      </c>
-      <c r="O20" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="79" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="80">
+      <c r="M20" s="81">
+        <v>0</v>
+      </c>
+      <c r="N20" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="79">
         <v>0.16</v>
       </c>
       <c r="E21" s="60">
@@ -2180,160 +2032,132 @@
       <c r="F21" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H21" s="81">
+      <c r="H21" s="80">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I21" s="81">
+      <c r="I21" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J21" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K21" s="82">
-        <v>0</v>
-      </c>
-      <c r="L21" s="83">
+      <c r="J21" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K21" s="81">
+        <v>0</v>
+      </c>
+      <c r="L21" s="82">
         <f>J21-K21</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M21" s="82">
-        <v>0</v>
-      </c>
-      <c r="N21" s="82">
-        <v>0</v>
-      </c>
-      <c r="O21" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M21" s="81">
+        <v>0</v>
+      </c>
+      <c r="N21" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E22" s="60">
         <v>6</v>
       </c>
       <c r="F22" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H22" s="81">
+      <c r="H22" s="80">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I22" s="81">
+      <c r="I22" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J22" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K22" s="82">
-        <v>0</v>
-      </c>
-      <c r="L22" s="83">
+      <c r="J22" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K22" s="81">
+        <v>0</v>
+      </c>
+      <c r="L22" s="82">
         <f>J22-K22</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M22" s="82">
-        <v>0</v>
-      </c>
-      <c r="N22" s="82">
-        <v>0</v>
-      </c>
-      <c r="O22" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M22" s="81">
+        <v>0</v>
+      </c>
+      <c r="N22" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E23" s="60">
         <v>5</v>
       </c>
       <c r="F23" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H23" s="81">
+      <c r="H23" s="80">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I23" s="81">
+      <c r="I23" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J23" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K23" s="82">
-        <v>0</v>
-      </c>
-      <c r="L23" s="83">
+      <c r="J23" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K23" s="81">
+        <v>0</v>
+      </c>
+      <c r="L23" s="82">
         <f>J23-K23</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M23" s="82">
-        <v>0</v>
-      </c>
-      <c r="N23" s="82">
-        <v>0</v>
-      </c>
-      <c r="O23" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M23" s="81">
+        <v>0</v>
+      </c>
+      <c r="N23" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E24" s="60">
         <v>4</v>
       </c>
       <c r="F24" s="61">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H24" s="81">
+      <c r="H24" s="80">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I24" s="81">
+      <c r="I24" s="80">
         <f>$C$20</f>
         <v>0.16</v>
       </c>
-      <c r="J24" s="82">
-        <v>410.20299999999997</v>
-      </c>
-      <c r="K24" s="82">
-        <v>0</v>
-      </c>
-      <c r="L24" s="83">
+      <c r="J24" s="81">
+        <v>410.20299999999997</v>
+      </c>
+      <c r="K24" s="81">
+        <v>0</v>
+      </c>
+      <c r="L24" s="82">
         <f>J24-K24</f>
         <v>410.20299999999997</v>
       </c>
-      <c r="M24" s="82">
-        <v>0</v>
-      </c>
-      <c r="N24" s="82">
-        <v>0</v>
-      </c>
-      <c r="O24" s="84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="73">
-        <f t="shared" si="2"/>
-        <v>199.76886100000002</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M24" s="81">
+        <v>0</v>
+      </c>
+      <c r="N24" s="83">
+        <f t="shared" si="1"/>
+        <v>199.76886099999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E25" s="60">
         <v>3</v>
       </c>
@@ -2361,19 +2185,12 @@
       <c r="M25" s="70">
         <v>0</v>
       </c>
-      <c r="N25" s="70">
-        <v>0</v>
-      </c>
-      <c r="O25" s="72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="73">
-        <f t="shared" si="2"/>
+      <c r="N25" s="72">
+        <f t="shared" si="1"/>
         <v>200.01187400000001</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E26" s="60">
         <v>2</v>
       </c>
@@ -2401,19 +2218,12 @@
       <c r="M26" s="70">
         <v>255.92599999999999</v>
       </c>
-      <c r="N26" s="70">
-        <v>0</v>
-      </c>
-      <c r="O26" s="72">
-        <f t="shared" si="1"/>
-        <v>255.92599999999999</v>
-      </c>
-      <c r="P26" s="73">
-        <f t="shared" si="2"/>
+      <c r="N26" s="72">
+        <f t="shared" si="1"/>
         <v>188.83676300000002</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="E27" s="60">
         <v>1</v>
       </c>
@@ -2435,25 +2245,18 @@
         <v>0</v>
       </c>
       <c r="L27" s="71">
-        <f t="shared" ref="L27:L28" si="3">J27-K27</f>
+        <f t="shared" ref="L27:L28" si="2">J27-K27</f>
         <v>205.286</v>
       </c>
       <c r="M27" s="70">
         <v>514.17600000000004</v>
       </c>
-      <c r="N27" s="70">
-        <v>0</v>
-      </c>
-      <c r="O27" s="72">
-        <f t="shared" si="1"/>
-        <v>514.17600000000004</v>
-      </c>
-      <c r="P27" s="73">
-        <f t="shared" si="2"/>
+      <c r="N27" s="72">
+        <f t="shared" si="1"/>
         <v>323.63123200000001</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="66">
         <v>-1</v>
       </c>
@@ -2470,32 +2273,23 @@
         <v>0</v>
       </c>
       <c r="L28" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M28" s="69"/>
-      <c r="N28" s="69">
-        <v>0</v>
-      </c>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="O29" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="P29" s="91">
-        <f>SUM(P4:P27)</f>
-        <v>4741.3130150000006</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="O30" s="90"/>
-      <c r="P30" s="90"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="O31" s="90"/>
-      <c r="P31" s="90"/>
+      <c r="N28" s="69"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N29" s="88">
+        <f>SUM(N4:N27)</f>
+        <v>4741.3130149999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N30" s="87"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N31" s="87"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2547,7 +2341,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Termina cubicación plano muros
</commit_message>
<xml_diff>
--- a/Tarea 03/Cubicaciones.xlsx
+++ b/Tarea 03/Cubicaciones.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FBDF130F-C36D-41B4-97F9-4BC06B17B396}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{36DEF1FE-2972-4B25-904F-47760E4F0A46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cubicaciones" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Distancias muros" sheetId="3" r:id="rId2"/>
     <sheet name="Verificación corte muros" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
@@ -152,6 +152,89 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{4749D284-6B11-4B4E-8FD3-458814A0AADE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Muro debajo del estacionamiento piso 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{DF4F64D8-C572-4D8A-8C5E-49ECF22C8E36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pilares eje 17??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J28" authorId="0" shapeId="0" xr:uid="{8F695FF7-2978-472F-B97C-A02D6F11663A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pilares eje 17
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
@@ -3002,11 +3085,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3272EE64-BB1C-472D-9C2F-0E5132DDD9CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3272EE64-BB1C-472D-9C2F-0E5132DDD9CA}">
   <dimension ref="A1:M647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="K30" sqref="K28:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3074,27 +3157,27 @@
       </c>
       <c r="F4" s="97">
         <f>SUM(F5:F54)</f>
-        <v>0</v>
+        <v>50.47999999999999</v>
       </c>
       <c r="G4" s="97">
         <f>SUM(G5:G54)</f>
-        <v>0</v>
+        <v>65.349999999999994</v>
       </c>
       <c r="H4" s="23">
         <f>SUM(H5:H54)</f>
-        <v>0</v>
+        <v>54.98</v>
       </c>
       <c r="I4" s="20">
         <f>SUM(I5:I54)</f>
-        <v>0</v>
+        <v>69.97999999999999</v>
       </c>
       <c r="J4" s="97">
         <f>SUM(J5:J54)</f>
-        <v>0</v>
+        <v>61.529999999999987</v>
       </c>
       <c r="K4" s="97">
         <f>SUM(K5:K54)</f>
-        <v>0</v>
+        <v>78.44</v>
       </c>
       <c r="L4" s="23">
         <f>SUM(L5:L54)</f>
@@ -3156,12 +3239,24 @@
       <c r="E6" s="103">
         <v>1.71</v>
       </c>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
+      <c r="F6" s="102">
+        <v>2.6</v>
+      </c>
+      <c r="G6" s="102">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="103">
+        <v>1.4</v>
+      </c>
+      <c r="I6" s="103">
+        <v>7.16</v>
+      </c>
+      <c r="J6" s="102">
+        <v>5.3</v>
+      </c>
+      <c r="K6" s="102">
+        <v>5.34</v>
+      </c>
       <c r="L6" s="103">
         <v>4</v>
       </c>
@@ -3182,12 +3277,24 @@
       <c r="E7" s="103">
         <v>0.7</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
+      <c r="F7" s="102">
+        <v>3.4</v>
+      </c>
+      <c r="G7" s="102">
+        <v>0.7</v>
+      </c>
+      <c r="H7" s="103">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="103">
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="102">
+        <v>2.57</v>
+      </c>
+      <c r="K7" s="102">
+        <v>1.52</v>
+      </c>
       <c r="L7" s="103">
         <v>2.2999999999999998</v>
       </c>
@@ -3208,12 +3315,24 @@
       <c r="E8" s="103">
         <v>0.7</v>
       </c>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
+      <c r="F8" s="102">
+        <v>2</v>
+      </c>
+      <c r="G8" s="102">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="103">
+        <v>2.6</v>
+      </c>
+      <c r="I8" s="103">
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="102">
+        <v>2.57</v>
+      </c>
+      <c r="K8" s="102">
+        <v>4.3</v>
+      </c>
       <c r="L8" s="103">
         <v>4.8</v>
       </c>
@@ -3234,12 +3353,24 @@
       <c r="E9" s="103">
         <v>0.6</v>
       </c>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
+      <c r="F9" s="102">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="102">
+        <v>0.7</v>
+      </c>
+      <c r="H9" s="103">
+        <v>2</v>
+      </c>
+      <c r="I9" s="103">
+        <v>0.6</v>
+      </c>
+      <c r="J9" s="102">
+        <v>3.9</v>
+      </c>
+      <c r="K9" s="102">
+        <v>1.92</v>
+      </c>
       <c r="L9" s="103">
         <v>0.85</v>
       </c>
@@ -3260,12 +3391,24 @@
       <c r="E10" s="103">
         <v>0.6</v>
       </c>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="102"/>
+      <c r="F10" s="102">
+        <v>2</v>
+      </c>
+      <c r="G10" s="102">
+        <v>0.6</v>
+      </c>
+      <c r="H10" s="103">
+        <v>2.8</v>
+      </c>
+      <c r="I10" s="103">
+        <v>0.7</v>
+      </c>
+      <c r="J10" s="102">
+        <v>1.67</v>
+      </c>
+      <c r="K10" s="102">
+        <v>1.6</v>
+      </c>
       <c r="L10" s="103">
         <v>0.85</v>
       </c>
@@ -3286,12 +3429,24 @@
       <c r="E11" s="103">
         <v>3.38</v>
       </c>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
+      <c r="F11" s="102">
+        <v>2.86</v>
+      </c>
+      <c r="G11" s="102">
+        <v>0.6</v>
+      </c>
+      <c r="H11" s="103">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I11" s="103">
+        <v>0.7</v>
+      </c>
+      <c r="J11" s="102">
+        <v>6.38</v>
+      </c>
+      <c r="K11" s="102">
+        <v>2.08</v>
+      </c>
       <c r="L11" s="103">
         <v>0.8</v>
       </c>
@@ -3312,12 +3467,24 @@
       <c r="E12" s="103">
         <v>1.5</v>
       </c>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
+      <c r="F12" s="102">
+        <v>5.35</v>
+      </c>
+      <c r="G12" s="102">
+        <v>1.92</v>
+      </c>
+      <c r="H12" s="103">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="103">
+        <v>0.7</v>
+      </c>
+      <c r="J12" s="102">
+        <v>2.67</v>
+      </c>
+      <c r="K12" s="102">
+        <v>5</v>
+      </c>
       <c r="L12" s="103">
         <v>2</v>
       </c>
@@ -3336,12 +3503,24 @@
       <c r="E13" s="103">
         <v>4.45</v>
       </c>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
+      <c r="F13" s="102">
+        <v>4</v>
+      </c>
+      <c r="G13" s="102">
+        <v>4.8</v>
+      </c>
+      <c r="H13" s="103">
+        <v>2</v>
+      </c>
+      <c r="I13" s="103">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J13" s="102">
+        <v>0.85</v>
+      </c>
+      <c r="K13" s="102">
+        <v>4.43</v>
+      </c>
       <c r="L13" s="103">
         <v>2</v>
       </c>
@@ -3360,12 +3539,24 @@
       <c r="E14" s="103">
         <v>6.35</v>
       </c>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
+      <c r="F14" s="102">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G14" s="102">
+        <v>3.7</v>
+      </c>
+      <c r="H14" s="103">
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="103">
+        <v>0.95</v>
+      </c>
+      <c r="J14" s="102">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="102">
+        <v>1.92</v>
+      </c>
       <c r="L14" s="103"/>
       <c r="M14" s="103"/>
     </row>
@@ -3382,12 +3573,24 @@
       <c r="E15" s="103">
         <v>6.15</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="102"/>
+      <c r="F15" s="102">
+        <v>4.8</v>
+      </c>
+      <c r="G15" s="102">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H15" s="103">
+        <v>2.73</v>
+      </c>
+      <c r="I15" s="103">
+        <v>1.92</v>
+      </c>
+      <c r="J15" s="102">
+        <v>4</v>
+      </c>
+      <c r="K15" s="102">
+        <v>1.92</v>
+      </c>
       <c r="L15" s="103"/>
       <c r="M15" s="103"/>
     </row>
@@ -3404,12 +3607,24 @@
       <c r="E16" s="103">
         <v>3.8</v>
       </c>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
+      <c r="F16" s="102">
+        <v>0.85</v>
+      </c>
+      <c r="G16" s="102">
+        <v>5.16</v>
+      </c>
+      <c r="H16" s="103">
+        <v>2</v>
+      </c>
+      <c r="I16" s="103">
+        <v>4.42</v>
+      </c>
+      <c r="J16" s="102">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K16" s="102">
+        <v>2.6</v>
+      </c>
       <c r="L16" s="103"/>
       <c r="M16" s="103"/>
     </row>
@@ -3426,12 +3641,24 @@
       <c r="E17" s="103">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
+      <c r="F17" s="102">
+        <v>2</v>
+      </c>
+      <c r="G17" s="102">
+        <v>3.84</v>
+      </c>
+      <c r="H17" s="103">
+        <v>4</v>
+      </c>
+      <c r="I17" s="103">
+        <v>1.2</v>
+      </c>
+      <c r="J17" s="102">
+        <v>4.8</v>
+      </c>
+      <c r="K17" s="102">
+        <v>3.24</v>
+      </c>
       <c r="L17" s="103"/>
       <c r="M17" s="103"/>
     </row>
@@ -3448,12 +3675,24 @@
       <c r="E18" s="103">
         <v>6.15</v>
       </c>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="102"/>
+      <c r="F18" s="102">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G18" s="102">
+        <v>1.18</v>
+      </c>
+      <c r="H18" s="103">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I18" s="103">
+        <v>3.79</v>
+      </c>
+      <c r="J18" s="102">
+        <v>2</v>
+      </c>
+      <c r="K18" s="102">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="L18" s="103"/>
       <c r="M18" s="103"/>
     </row>
@@ -3470,12 +3709,24 @@
       <c r="E19" s="103">
         <v>4.45</v>
       </c>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="102"/>
+      <c r="F19" s="102">
+        <v>0.8</v>
+      </c>
+      <c r="G19" s="102">
+        <v>6.15</v>
+      </c>
+      <c r="H19" s="103">
+        <v>4.8</v>
+      </c>
+      <c r="I19" s="103">
+        <v>1.18</v>
+      </c>
+      <c r="J19" s="102">
+        <v>8.43</v>
+      </c>
+      <c r="K19" s="102">
+        <v>4.92</v>
+      </c>
       <c r="L19" s="103"/>
       <c r="M19" s="103"/>
     </row>
@@ -3492,12 +3743,24 @@
       <c r="E20" s="103">
         <v>1.5</v>
       </c>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="103"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
+      <c r="F20" s="102">
+        <v>5.5</v>
+      </c>
+      <c r="G20" s="102">
+        <v>4.43</v>
+      </c>
+      <c r="H20" s="103">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="I20" s="103">
+        <v>6.1</v>
+      </c>
+      <c r="J20" s="102">
+        <v>0.85</v>
+      </c>
+      <c r="K20" s="102">
+        <v>6.18</v>
+      </c>
       <c r="L20" s="103"/>
       <c r="M20" s="103"/>
     </row>
@@ -3514,12 +3777,24 @@
       <c r="E21" s="103">
         <v>3.38</v>
       </c>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="102"/>
-      <c r="K21" s="102"/>
+      <c r="F21" s="102">
+        <v>0.62</v>
+      </c>
+      <c r="G21" s="102">
+        <v>1.19</v>
+      </c>
+      <c r="H21" s="103">
+        <v>0.85</v>
+      </c>
+      <c r="I21" s="103">
+        <v>5.14</v>
+      </c>
+      <c r="J21" s="102">
+        <v>1.02</v>
+      </c>
+      <c r="K21" s="102">
+        <v>3.82</v>
+      </c>
       <c r="L21" s="103"/>
       <c r="M21" s="103"/>
     </row>
@@ -3536,12 +3811,24 @@
       <c r="E22" s="103">
         <v>0.6</v>
       </c>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="103"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
+      <c r="F22" s="102">
+        <v>0.62</v>
+      </c>
+      <c r="G22" s="102">
+        <v>3.38</v>
+      </c>
+      <c r="H22" s="103">
+        <v>1</v>
+      </c>
+      <c r="I22" s="103">
+        <v>4.41</v>
+      </c>
+      <c r="J22" s="102">
+        <v>2.8</v>
+      </c>
+      <c r="K22" s="102">
+        <v>1.2</v>
+      </c>
       <c r="L22" s="103"/>
       <c r="M22" s="103"/>
     </row>
@@ -3558,12 +3845,24 @@
       <c r="E23" s="103">
         <v>0.6</v>
       </c>
-      <c r="F23" s="102"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="102"/>
+      <c r="F23" s="102">
+        <v>2.62</v>
+      </c>
+      <c r="G23" s="102">
+        <v>0.6</v>
+      </c>
+      <c r="H23" s="103">
+        <v>2.75</v>
+      </c>
+      <c r="I23" s="103">
+        <v>1.92</v>
+      </c>
+      <c r="J23" s="102">
+        <v>5.52</v>
+      </c>
+      <c r="K23" s="102">
+        <v>6.15</v>
+      </c>
       <c r="L23" s="103"/>
       <c r="M23" s="103"/>
     </row>
@@ -3580,12 +3879,24 @@
       <c r="E24" s="103">
         <v>2.78</v>
       </c>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="102"/>
+      <c r="F24" s="102">
+        <v>1.56</v>
+      </c>
+      <c r="G24" s="102">
+        <v>0.6</v>
+      </c>
+      <c r="H24" s="103">
+        <v>5.5</v>
+      </c>
+      <c r="I24" s="103">
+        <v>1.92</v>
+      </c>
+      <c r="J24" s="102">
+        <v>0.8</v>
+      </c>
+      <c r="K24" s="102">
+        <v>5</v>
+      </c>
       <c r="L24" s="103"/>
       <c r="M24" s="103"/>
     </row>
@@ -3602,12 +3913,24 @@
       <c r="E25" s="103">
         <v>0.4</v>
       </c>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="103"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="102"/>
+      <c r="F25" s="102">
+        <v>1.4</v>
+      </c>
+      <c r="G25" s="102">
+        <v>1.92</v>
+      </c>
+      <c r="H25" s="103">
+        <v>0.8</v>
+      </c>
+      <c r="I25" s="103">
+        <v>0.6</v>
+      </c>
+      <c r="J25" s="102">
+        <v>0.8</v>
+      </c>
+      <c r="K25" s="102">
+        <v>0.53</v>
+      </c>
       <c r="L25" s="103"/>
       <c r="M25" s="103"/>
     </row>
@@ -3625,11 +3948,21 @@
         <v>1.72</v>
       </c>
       <c r="F26" s="102"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="103"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102"/>
+      <c r="G26" s="102">
+        <v>1.92</v>
+      </c>
+      <c r="H26" s="103">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="103">
+        <v>0.6</v>
+      </c>
+      <c r="J26" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="102">
+        <v>1.77</v>
+      </c>
       <c r="L26" s="103"/>
       <c r="M26" s="103"/>
     </row>
@@ -3647,11 +3980,21 @@
         <v>0.7</v>
       </c>
       <c r="F27" s="102"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="103"/>
-      <c r="J27" s="102"/>
-      <c r="K27" s="102"/>
+      <c r="G27" s="102">
+        <v>5.25</v>
+      </c>
+      <c r="H27" s="103">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="103">
+        <v>4.83</v>
+      </c>
+      <c r="J27" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="102">
+        <v>8.1</v>
+      </c>
       <c r="L27" s="103"/>
       <c r="M27" s="103"/>
     </row>
@@ -3665,10 +4008,18 @@
         <v>0.7</v>
       </c>
       <c r="F28" s="102"/>
-      <c r="G28" s="102"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="102"/>
+      <c r="G28" s="102">
+        <v>5.03</v>
+      </c>
+      <c r="H28" s="103">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="103">
+        <v>3.4</v>
+      </c>
+      <c r="J28" s="102">
+        <v>0.5</v>
+      </c>
       <c r="K28" s="102"/>
       <c r="L28" s="103"/>
       <c r="M28" s="103"/>
@@ -3683,9 +4034,13 @@
         <v>0.4</v>
       </c>
       <c r="F29" s="102"/>
-      <c r="G29" s="102"/>
+      <c r="G29" s="102">
+        <v>1.3</v>
+      </c>
       <c r="H29" s="103"/>
-      <c r="I29" s="103"/>
+      <c r="I29" s="103">
+        <v>5.27</v>
+      </c>
       <c r="J29" s="102"/>
       <c r="K29" s="102"/>
       <c r="L29" s="103"/>
@@ -3699,9 +4054,13 @@
         <v>1.92</v>
       </c>
       <c r="F30" s="102"/>
-      <c r="G30" s="102"/>
+      <c r="G30" s="102">
+        <v>0.4</v>
+      </c>
       <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
+      <c r="I30" s="103">
+        <v>6.57</v>
+      </c>
       <c r="J30" s="102"/>
       <c r="K30" s="102"/>
       <c r="L30" s="103"/>
@@ -3715,7 +4074,9 @@
         <v>1.92</v>
       </c>
       <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
+      <c r="G31" s="102">
+        <v>2.8</v>
+      </c>
       <c r="H31" s="103"/>
       <c r="I31" s="103"/>
       <c r="J31" s="102"/>
@@ -3729,7 +4090,9 @@
       <c r="D32" s="103"/>
       <c r="E32" s="103"/>
       <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
+      <c r="G32" s="102">
+        <v>4.92</v>
+      </c>
       <c r="H32" s="103"/>
       <c r="I32" s="103"/>
       <c r="J32" s="102"/>
@@ -12357,6 +12720,7 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12365,7 +12729,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modificada tabla resumen y agregado excel con tablas latex
</commit_message>
<xml_diff>
--- a/Tarea 03/Cubicaciones.xlsx
+++ b/Tarea 03/Cubicaciones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BD012E-E90E-4849-9656-5F0FF6D7A916}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C8D7BC-2418-47F5-8142-548140844175}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cubicaciones" sheetId="5" r:id="rId1"/>
@@ -2556,6 +2556,51 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2583,27 +2628,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2627,30 +2651,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2949,8 +2949,8 @@
   </sheetPr>
   <dimension ref="B2:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2980,31 +2980,31 @@
       <c r="F2" s="171" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="238" t="s">
+      <c r="G2" s="214" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="238" t="s">
+      <c r="H2" s="214" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="238" t="s">
+      <c r="I2" s="214" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="238" t="s">
+      <c r="J2" s="214" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="238" t="s">
+      <c r="K2" s="214" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="238" t="s">
+      <c r="L2" s="214" t="s">
         <v>124</v>
       </c>
-      <c r="M2" s="238" t="s">
+      <c r="M2" s="214" t="s">
         <v>128</v>
       </c>
-      <c r="N2" s="238" t="s">
+      <c r="N2" s="214" t="s">
         <v>129</v>
       </c>
-      <c r="O2" s="238" t="s">
+      <c r="O2" s="214" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3034,7 +3034,7 @@
         <f>'Pesos elementos'!T4</f>
         <v>209.70329500000003</v>
       </c>
-      <c r="M3" s="245">
+      <c r="M3" s="220">
         <f>L3/9.8</f>
         <v>21.398295408163268</v>
       </c>
@@ -3073,7 +3073,7 @@
         <f>'Pesos elementos'!T5</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M4" s="245">
+      <c r="M4" s="220">
         <f t="shared" ref="M4:M26" si="0">L4/9.8</f>
         <v>47.819172959183675</v>
       </c>
@@ -3112,7 +3112,7 @@
         <f>'Pesos elementos'!T6</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M5" s="245">
+      <c r="M5" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3151,7 +3151,7 @@
         <f>'Pesos elementos'!T7</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M6" s="245">
+      <c r="M6" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3190,7 +3190,7 @@
         <f>'Pesos elementos'!T8</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M7" s="245">
+      <c r="M7" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3229,7 +3229,7 @@
         <f>'Pesos elementos'!T9</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M8" s="245">
+      <c r="M8" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3268,7 +3268,7 @@
         <f>'Pesos elementos'!T10</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M9" s="245">
+      <c r="M9" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3307,7 +3307,7 @@
         <f>'Pesos elementos'!T11</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M10" s="245">
+      <c r="M10" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3346,7 +3346,7 @@
         <f>'Pesos elementos'!T12</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M11" s="245">
+      <c r="M11" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3385,7 +3385,7 @@
         <f>'Pesos elementos'!T13</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M12" s="245">
+      <c r="M12" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3424,7 +3424,7 @@
         <f>'Pesos elementos'!T14</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M13" s="245">
+      <c r="M13" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3463,7 +3463,7 @@
         <f>'Pesos elementos'!T15</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M14" s="245">
+      <c r="M14" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3502,7 +3502,7 @@
         <f>'Pesos elementos'!T16</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M15" s="245">
+      <c r="M15" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3541,7 +3541,7 @@
         <f>'Pesos elementos'!T17</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M16" s="245">
+      <c r="M16" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3580,7 +3580,7 @@
         <f>'Pesos elementos'!T18</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M17" s="245">
+      <c r="M17" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3619,7 +3619,7 @@
         <f>'Pesos elementos'!T19</f>
         <v>468.62789500000002</v>
       </c>
-      <c r="M18" s="245">
+      <c r="M18" s="220">
         <f t="shared" si="0"/>
         <v>47.819172959183675</v>
       </c>
@@ -3658,7 +3658,7 @@
         <f>'Pesos elementos'!T20</f>
         <v>476.45945750000004</v>
       </c>
-      <c r="M19" s="245">
+      <c r="M19" s="220">
         <f t="shared" si="0"/>
         <v>48.61831198979592</v>
       </c>
@@ -3697,7 +3697,7 @@
         <f>'Pesos elementos'!T21</f>
         <v>492.7522075</v>
       </c>
-      <c r="M20" s="245">
+      <c r="M20" s="220">
         <f t="shared" si="0"/>
         <v>50.280837499999997</v>
       </c>
@@ -3736,7 +3736,7 @@
         <f>'Pesos elementos'!T22</f>
         <v>501.46251999999998</v>
       </c>
-      <c r="M21" s="245">
+      <c r="M21" s="220">
         <f t="shared" si="0"/>
         <v>51.169644897959181</v>
       </c>
@@ -3775,7 +3775,7 @@
         <f>'Pesos elementos'!T23</f>
         <v>501.71164499999998</v>
       </c>
-      <c r="M22" s="245">
+      <c r="M22" s="220">
         <f t="shared" si="0"/>
         <v>51.195065816326526</v>
       </c>
@@ -3814,7 +3814,7 @@
         <f>'Pesos elementos'!T24</f>
         <v>504.47644500000001</v>
       </c>
-      <c r="M23" s="245">
+      <c r="M23" s="220">
         <f t="shared" si="0"/>
         <v>51.477188265306118</v>
       </c>
@@ -3853,7 +3853,7 @@
         <f>'Pesos elementos'!T25</f>
         <v>513.04554250000001</v>
       </c>
-      <c r="M24" s="245">
+      <c r="M24" s="220">
         <f t="shared" si="0"/>
         <v>52.351585969387756</v>
       </c>
@@ -3892,7 +3892,7 @@
         <f>'Pesos elementos'!T26</f>
         <v>511.21057999999999</v>
       </c>
-      <c r="M25" s="245">
+      <c r="M25" s="220">
         <f t="shared" si="0"/>
         <v>52.164344897959182</v>
       </c>
@@ -3931,7 +3931,7 @@
         <f>'Pesos elementos'!T27</f>
         <v>729.26028500000007</v>
       </c>
-      <c r="M26" s="245">
+      <c r="M26" s="220">
         <f t="shared" si="0"/>
         <v>74.414314795918372</v>
       </c>
@@ -3964,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" topLeftCell="F38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5744,48 +5744,48 @@
       <c r="N31" s="77"/>
     </row>
     <row r="32" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="217" t="s">
+      <c r="H32" s="232" t="s">
         <v>34</v>
       </c>
-      <c r="I32" s="214" t="s">
+      <c r="I32" s="229" t="s">
         <v>59</v>
       </c>
-      <c r="J32" s="215"/>
-      <c r="K32" s="215"/>
-      <c r="L32" s="216"/>
+      <c r="J32" s="230"/>
+      <c r="K32" s="230"/>
+      <c r="L32" s="231"/>
       <c r="M32" s="225" t="s">
         <v>58</v>
       </c>
       <c r="N32" s="226"/>
       <c r="O32" s="226"/>
       <c r="P32" s="227"/>
-      <c r="Q32" s="228" t="s">
+      <c r="Q32" s="221" t="s">
         <v>62</v>
       </c>
-      <c r="R32" s="228" t="s">
+      <c r="R32" s="221" t="s">
         <v>74</v>
       </c>
-      <c r="S32" s="228" t="s">
+      <c r="S32" s="221" t="s">
         <v>63</v>
       </c>
-      <c r="T32" s="219" t="s">
+      <c r="T32" s="234" t="s">
         <v>61</v>
       </c>
-      <c r="U32" s="221" t="s">
+      <c r="U32" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="V32" s="221" t="s">
+      <c r="V32" s="236" t="s">
         <v>73</v>
       </c>
       <c r="W32" s="223" t="s">
         <v>75</v>
       </c>
-      <c r="X32" s="228" t="s">
+      <c r="X32" s="221" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="33" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H33" s="218"/>
+      <c r="H33" s="233"/>
       <c r="I33" s="105" t="s">
         <v>13</v>
       </c>
@@ -5810,14 +5810,14 @@
       <c r="P33" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="Q33" s="229"/>
-      <c r="R33" s="229"/>
-      <c r="S33" s="229"/>
-      <c r="T33" s="220"/>
-      <c r="U33" s="222"/>
-      <c r="V33" s="222"/>
+      <c r="Q33" s="228"/>
+      <c r="R33" s="228"/>
+      <c r="S33" s="228"/>
+      <c r="T33" s="235"/>
+      <c r="U33" s="237"/>
+      <c r="V33" s="237"/>
       <c r="W33" s="224"/>
-      <c r="X33" s="243"/>
+      <c r="X33" s="222"/>
     </row>
     <row r="34" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H34" s="101">
@@ -5878,11 +5878,11 @@
         <f t="shared" ref="V34:V58" si="17">R34*$C$16*$C$5</f>
         <v>0.11255</v>
       </c>
-      <c r="W34" s="239">
+      <c r="W34" s="215">
         <f>T34+U34+V34</f>
         <v>51.68954999999999</v>
       </c>
-      <c r="X34" s="244">
+      <c r="X34" s="219">
         <f>T34+V34</f>
         <v>51.310549999999992</v>
       </c>
@@ -5946,7 +5946,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W35" s="240">
+      <c r="W35" s="216">
         <f t="shared" ref="W35:W58" si="20">T35+U35+V35</f>
         <v>132.61860000000001</v>
       </c>
@@ -6014,7 +6014,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W36" s="240">
+      <c r="W36" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6082,7 +6082,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W37" s="240">
+      <c r="W37" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6150,7 +6150,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W38" s="240">
+      <c r="W38" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6218,7 +6218,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W39" s="240">
+      <c r="W39" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6286,7 +6286,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W40" s="240">
+      <c r="W40" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6354,7 +6354,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W41" s="240">
+      <c r="W41" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6422,7 +6422,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W42" s="240">
+      <c r="W42" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6490,7 +6490,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W43" s="240">
+      <c r="W43" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6558,7 +6558,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W44" s="240">
+      <c r="W44" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6626,7 +6626,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W45" s="240">
+      <c r="W45" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6694,7 +6694,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W46" s="240">
+      <c r="W46" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6762,7 +6762,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W47" s="240">
+      <c r="W47" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6830,7 +6830,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W48" s="240">
+      <c r="W48" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6898,7 +6898,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W49" s="240">
+      <c r="W49" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -6966,7 +6966,7 @@
         <f t="shared" si="17"/>
         <v>0.28460000000000008</v>
       </c>
-      <c r="W50" s="240">
+      <c r="W50" s="216">
         <f t="shared" si="20"/>
         <v>132.61860000000001</v>
       </c>
@@ -7034,7 +7034,7 @@
         <f t="shared" si="17"/>
         <v>0.28472500000000006</v>
       </c>
-      <c r="W51" s="240">
+      <c r="W51" s="216">
         <f t="shared" si="20"/>
         <v>148.28172500000002</v>
       </c>
@@ -7102,7 +7102,7 @@
         <f t="shared" si="17"/>
         <v>0.28485000000000005</v>
       </c>
-      <c r="W52" s="240">
+      <c r="W52" s="216">
         <f t="shared" si="20"/>
         <v>165.20409999999998</v>
       </c>
@@ -7170,7 +7170,7 @@
         <f t="shared" si="17"/>
         <v>0.28485000000000005</v>
       </c>
-      <c r="W53" s="240">
+      <c r="W53" s="216">
         <f t="shared" si="20"/>
         <v>165.70235</v>
       </c>
@@ -7238,7 +7238,7 @@
         <f t="shared" si="17"/>
         <v>0.28485000000000005</v>
       </c>
-      <c r="W54" s="240">
+      <c r="W54" s="216">
         <f t="shared" si="20"/>
         <v>165.70235</v>
       </c>
@@ -7306,7 +7306,7 @@
         <f t="shared" si="17"/>
         <v>0.29445000000000005</v>
       </c>
-      <c r="W55" s="241">
+      <c r="W55" s="217">
         <f t="shared" si="20"/>
         <v>171.23195000000004</v>
       </c>
@@ -7374,7 +7374,7 @@
         <f t="shared" si="17"/>
         <v>0.29119999999999996</v>
       </c>
-      <c r="W56" s="241">
+      <c r="W56" s="217">
         <f t="shared" si="20"/>
         <v>183.37257499999996</v>
       </c>
@@ -7442,7 +7442,7 @@
         <f t="shared" si="17"/>
         <v>0.314025</v>
       </c>
-      <c r="W57" s="241">
+      <c r="W57" s="217">
         <f t="shared" si="20"/>
         <v>197.65272499999995</v>
       </c>
@@ -7510,7 +7510,7 @@
         <f t="shared" si="17"/>
         <v>0.35154999999999997</v>
       </c>
-      <c r="W58" s="242">
+      <c r="W58" s="218">
         <f t="shared" si="20"/>
         <v>220.32079999999996</v>
       </c>
@@ -8284,17 +8284,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="V32:V33"/>
     <mergeCell ref="X32:X33"/>
     <mergeCell ref="W32:W33"/>
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="Q32:Q33"/>
     <mergeCell ref="R32:R33"/>
     <mergeCell ref="S32:S33"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="V32:V33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8306,8 +8306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A282A9DD-DDA8-407B-9F67-055CDE136535}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19:T26"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9792,37 +9792,37 @@
       <c r="B1" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="230" t="s">
+      <c r="C1" s="238" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="232" t="s">
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="230" t="s">
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="238" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
-      <c r="N1" s="231"/>
-      <c r="O1" s="231"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="S1" s="232" t="s">
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
+      <c r="M1" s="239"/>
+      <c r="N1" s="239"/>
+      <c r="O1" s="239"/>
+      <c r="P1" s="239"/>
+      <c r="Q1" s="239"/>
+      <c r="S1" s="240" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="233"/>
-      <c r="U1" s="233"/>
-      <c r="V1" s="233"/>
-      <c r="W1" s="233"/>
-      <c r="X1" s="233"/>
-      <c r="Y1" s="233"/>
-      <c r="Z1" s="233"/>
+      <c r="T1" s="241"/>
+      <c r="U1" s="241"/>
+      <c r="V1" s="241"/>
+      <c r="W1" s="241"/>
+      <c r="X1" s="241"/>
+      <c r="Y1" s="241"/>
+      <c r="Z1" s="241"/>
       <c r="AA1" s="155"/>
     </row>
     <row r="2" spans="1:27" s="141" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16407,30 +16407,30 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="234" t="s">
+      <c r="B3" s="242" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="235"/>
-      <c r="D3" s="236" t="s">
+      <c r="C3" s="243"/>
+      <c r="D3" s="244" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="237"/>
-      <c r="F3" s="235" t="s">
+      <c r="E3" s="245"/>
+      <c r="F3" s="243" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="235"/>
-      <c r="H3" s="236" t="s">
+      <c r="G3" s="243"/>
+      <c r="H3" s="244" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="237"/>
-      <c r="J3" s="235" t="s">
+      <c r="I3" s="245"/>
+      <c r="J3" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="235"/>
-      <c r="L3" s="236" t="s">
+      <c r="K3" s="243"/>
+      <c r="L3" s="244" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="237"/>
+      <c r="M3" s="245"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -26050,30 +26050,30 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="234" t="s">
+      <c r="B3" s="242" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="235"/>
-      <c r="D3" s="236" t="s">
+      <c r="C3" s="243"/>
+      <c r="D3" s="244" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="237"/>
-      <c r="F3" s="235" t="s">
+      <c r="E3" s="245"/>
+      <c r="F3" s="243" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="235"/>
-      <c r="H3" s="236" t="s">
+      <c r="G3" s="243"/>
+      <c r="H3" s="244" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="237"/>
-      <c r="J3" s="235" t="s">
+      <c r="I3" s="245"/>
+      <c r="J3" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="235"/>
-      <c r="L3" s="236" t="s">
+      <c r="K3" s="243"/>
+      <c r="L3" s="244" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="237"/>
+      <c r="M3" s="245"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">

</xml_diff>